<commit_message>
Made it to the results
</commit_message>
<xml_diff>
--- a/Charts20160405.xlsx
+++ b/Charts20160405.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7740" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7740" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Environmental variables" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,13 @@
     <sheet name="Model selection" sheetId="2" r:id="rId4"/>
     <sheet name="Model selection-product" sheetId="5" r:id="rId5"/>
     <sheet name="H1 suitability" sheetId="9" r:id="rId6"/>
-    <sheet name="Significance" sheetId="8" r:id="rId7"/>
+    <sheet name="Slope-Aspect" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet3" sheetId="12" r:id="rId8"/>
+    <sheet name="Sheet4" sheetId="13" r:id="rId9"/>
+    <sheet name="Significance" sheetId="8" r:id="rId10"/>
+    <sheet name="OLI bands" sheetId="15" r:id="rId11"/>
+    <sheet name="VegIndices" sheetId="16" r:id="rId12"/>
+    <sheet name="Steps" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -136,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="317">
   <si>
     <t>Layer</t>
   </si>
@@ -700,6 +706,415 @@
   </si>
   <si>
     <t>Range overlap at lowest in H1</t>
+  </si>
+  <si>
+    <t>Recalculated value</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Scene ID</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>LC81290452015052LGN00</t>
+  </si>
+  <si>
+    <t>LC81300442015075LGN00</t>
+  </si>
+  <si>
+    <t>LC81300452015075LGN00</t>
+  </si>
+  <si>
+    <t>LC81310442015066LGN00</t>
+  </si>
+  <si>
+    <t>LC81310452015066LGN00</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Abreviation</t>
+  </si>
+  <si>
+    <t>Landsat 8</t>
+  </si>
+  <si>
+    <t>LS8</t>
+  </si>
+  <si>
+    <t>Operational Land Imager</t>
+  </si>
+  <si>
+    <t>OLI</t>
+  </si>
+  <si>
+    <t>Thermal Infrared Sensor</t>
+  </si>
+  <si>
+    <t>TIRS</t>
+  </si>
+  <si>
+    <t>Thing</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>Download Landsat8 tiles</t>
+  </si>
+  <si>
+    <t>Took out Bands 4 and 5</t>
+  </si>
+  <si>
+    <t>Calculated NDVI with Image Analysis tool</t>
+  </si>
+  <si>
+    <t>ArcGIS&gt;Window&gt;ImageAnalysis</t>
+  </si>
+  <si>
+    <t>NDVI is calculated first so there are no seems</t>
+  </si>
+  <si>
+    <t>Export each layer</t>
+  </si>
+  <si>
+    <t>Mosaic with ERDAS</t>
+  </si>
+  <si>
+    <t>Band 6</t>
+  </si>
+  <si>
+    <t>Clip to bounds</t>
+  </si>
+  <si>
+    <t>ArcToobox.DatamgmtTools.Raster.RasterProcessing.Clip</t>
+  </si>
+  <si>
+    <t>Set data frame to WGS1984</t>
+  </si>
+  <si>
+    <t>Export raster data</t>
+  </si>
+  <si>
+    <t>Spatial reference = data frame</t>
+  </si>
+  <si>
+    <t>Raster to ASCII</t>
+  </si>
+  <si>
+    <t>ConversionTools&gt;FromRaster&gt;RasterToASCII</t>
+  </si>
+  <si>
+    <t>Try 2</t>
+  </si>
+  <si>
+    <t>Mosaic with ERDAS 2015</t>
+  </si>
+  <si>
+    <t>Convert to WGS1984</t>
+  </si>
+  <si>
+    <t>Calculate NDVI</t>
+  </si>
+  <si>
+    <t>Image Analysis Window</t>
+  </si>
+  <si>
+    <t>Export to ASCII</t>
+  </si>
+  <si>
+    <t>AcrToolbox&gt;ConversionTools&gt;FromRaster&gt;RasterToASCII</t>
+  </si>
+  <si>
+    <t>Band 5</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Clipped\B5\B5_C_1</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\ACSII\B5.ASC</t>
+  </si>
+  <si>
+    <t>Band 4</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Clipped\B4\b4_c_1</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\ACSII\B4.ASC</t>
+  </si>
+  <si>
+    <t>Get ASTER tiles</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Clipped\DEM\DEM_C_2</t>
+  </si>
+  <si>
+    <t>Calculate Aspect</t>
+  </si>
+  <si>
+    <t>ArcToolbox&gt;SpatialAnalystTools&gt;Surface&gt;Aspect</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Clipped\Aspect\aspect</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>Calculate Slope - Percent rise and Z factor of 1</t>
+  </si>
+  <si>
+    <t>ArcToolbox&gt;SpatialAnalystTools&gt;Surface&gt;Slope</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Clipped\slope\slope</t>
+  </si>
+  <si>
+    <t>Contor 10m</t>
+  </si>
+  <si>
+    <t>Calculate contors</t>
+  </si>
+  <si>
+    <t>ArcToolbox&gt;SpatialAnalystTools&gt;Surface&gt;Contour</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Clipped\Contour\10m\con_10m.shp</t>
+  </si>
+  <si>
+    <t>Contor 30m</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Clipped\Contour\30m\con_30m.shp</t>
+  </si>
+  <si>
+    <t>Contor 50m</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Clipped\Contour\50m\con_50m.shp</t>
+  </si>
+  <si>
+    <t>Contor 100m</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Clipped\Contour\100m\con_100m.shp</t>
+  </si>
+  <si>
+    <t>Calculate distance to roads</t>
+  </si>
+  <si>
+    <t>ArcToolbox&gt;SpatialAnalystTools&gt;Distance&gt;EuclideanDistance</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Mosaic\Roads\EucDist\rds_ed_8</t>
+  </si>
+  <si>
+    <t>Environments&gt;change everything possible to be the same as ndvi.asc</t>
+  </si>
+  <si>
+    <t>Direction to roads</t>
+  </si>
+  <si>
+    <t>Calculate direction to roads</t>
+  </si>
+  <si>
+    <t>ArcToolbox&gt;SpatialAnalystTools&gt;Distance&gt;EuclideanDirection</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Mosaic\Roads\EucDir\rds_edir_1</t>
+  </si>
+  <si>
+    <t>Cost distance to roads-slope</t>
+  </si>
+  <si>
+    <t>Calculate cost distance to roads using the slope layer</t>
+  </si>
+  <si>
+    <t>ArcToolbox&gt;SpatialAnalystTools&gt;Distance&gt;CostDistance</t>
+  </si>
+  <si>
+    <t>D:\bsu017\Start\Mosaic\Roads\CostDist\rds_edir_1</t>
+  </si>
+  <si>
+    <t>Spectral band</t>
+  </si>
+  <si>
+    <r>
+      <t>Wavelength (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µm)</t>
+    </r>
+  </si>
+  <si>
+    <t>Resolution (m)</t>
+  </si>
+  <si>
+    <t>Band 1 - Coastal/Aerosol</t>
+  </si>
+  <si>
+    <t>0.433-0.453</t>
+  </si>
+  <si>
+    <t>Band 2 - Blue</t>
+  </si>
+  <si>
+    <t>0.450-0.515</t>
+  </si>
+  <si>
+    <t>Band 3 - Green</t>
+  </si>
+  <si>
+    <t>0.525-0.600</t>
+  </si>
+  <si>
+    <t>Band 4 - Red</t>
+  </si>
+  <si>
+    <t>0.630-0.680</t>
+  </si>
+  <si>
+    <t>Band 5 - Near Infrared</t>
+  </si>
+  <si>
+    <t>0.845-0.885</t>
+  </si>
+  <si>
+    <t>Band 6 - Short Wavelength Infrared</t>
+  </si>
+  <si>
+    <t>1.560-1.660</t>
+  </si>
+  <si>
+    <t>Band 7 - Short Wavelength Infrared</t>
+  </si>
+  <si>
+    <t>2.100-2.300</t>
+  </si>
+  <si>
+    <t>Band 8 - Panchromatic</t>
+  </si>
+  <si>
+    <t>0.500-0.680</t>
+  </si>
+  <si>
+    <t>Band 9 - Cirrus</t>
+  </si>
+  <si>
+    <t>1.360-1.390</t>
+  </si>
+  <si>
+    <t>Band 10 - Long Wavelength Infrared</t>
+  </si>
+  <si>
+    <t>10.30-11.30</t>
+  </si>
+  <si>
+    <t>Band 11 - Long Wavelength Infrared</t>
+  </si>
+  <si>
+    <t>11.50-12.50</t>
+  </si>
+  <si>
+    <t>Veg indices</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>Non-Linear vegetation Index (NLI)</t>
+  </si>
+  <si>
+    <t>((B5^2)-B4)/((B5^2)+B4)</t>
+  </si>
+  <si>
+    <t>don't think this one works</t>
+  </si>
+  <si>
+    <t>Re-normalised Difference Vegetation Index (RDVI)</t>
+  </si>
+  <si>
+    <r>
+      <t>(B5-B4)/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>√(B5+B4)</t>
+    </r>
+  </si>
+  <si>
+    <t>Modified Simple Ratio (MSR)</t>
+  </si>
+  <si>
+    <t>(B5/B4-1)/(√(B5/B4)+1)</t>
+  </si>
+  <si>
+    <t>Atmospherically Resistant Vegetation Index (ARVI)</t>
+  </si>
+  <si>
+    <t>(B5-2*B4+B2)/(B5+2*B4-B2)</t>
+  </si>
+  <si>
+    <t>This needs some work</t>
+  </si>
+  <si>
+    <t>B1+B2+B3+B4+B5+B6+B7</t>
+  </si>
+  <si>
+    <t>This might not be right check the formula</t>
+  </si>
+  <si>
+    <t>Tasseled Cap Transformation - greenness</t>
+  </si>
+  <si>
+    <t>(0.3029 * "b2.tif") + (0.2786 * "b3.tif") + (0.4733 * "b4.tif") + (0.5599 * "b5.tif") + (0.508 * "b6.tif") + (0.1872 * "b7.tif")</t>
+  </si>
+  <si>
+    <t>See Baig 2014</t>
+  </si>
+  <si>
+    <t>Tasseled Cap Transformation - brightness</t>
+  </si>
+  <si>
+    <t>(B2* "b2.tif") + (B3 * "b3.tif") + (B4 * "b4.tif") + (B5 * "b5.tif") + (B6 * "b6.tif") + (B7 * "b7.tif")</t>
+  </si>
+  <si>
+    <t>See Baig 2014 where BX is the number shown in table 2</t>
+  </si>
+  <si>
+    <t>Tasseled Cap Transformation - wetness</t>
+  </si>
+  <si>
+    <t>Tasseled Cap Transformation - 4</t>
+  </si>
+  <si>
+    <t>Tasseled Cap Transformation - 5</t>
+  </si>
+  <si>
+    <t>Tasseled Cap Transformation - 6</t>
   </si>
 </sst>
 </file>
@@ -709,7 +1124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -759,6 +1174,18 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -773,9 +1200,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -786,7 +1231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -805,6 +1250,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1815,11 +2275,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="299171360"/>
-        <c:axId val="299171752"/>
+        <c:axId val="466430280"/>
+        <c:axId val="466429888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="299171360"/>
+        <c:axId val="466430280"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1862,7 +2322,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299171752"/>
+        <c:crossAx val="466429888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1870,7 +2330,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="299171752"/>
+        <c:axId val="466429888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.98"/>
@@ -1923,7 +2383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299171360"/>
+        <c:crossAx val="466430280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3146,6 +3606,720 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B7" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>285</v>
+      </c>
+      <c r="B9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>287</v>
+      </c>
+      <c r="B10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>289</v>
+      </c>
+      <c r="B11" t="s">
+        <v>290</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>291</v>
+      </c>
+      <c r="B12" t="s">
+        <v>292</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7" t="s">
+        <v>308</v>
+      </c>
+      <c r="D7" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B8" t="s">
+        <v>311</v>
+      </c>
+      <c r="D8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>313</v>
+      </c>
+      <c r="B9" t="s">
+        <v>311</v>
+      </c>
+      <c r="D9" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>314</v>
+      </c>
+      <c r="B10" t="s">
+        <v>311</v>
+      </c>
+      <c r="D10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>315</v>
+      </c>
+      <c r="B11" t="s">
+        <v>311</v>
+      </c>
+      <c r="D11" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>316</v>
+      </c>
+      <c r="B12" t="s">
+        <v>311</v>
+      </c>
+      <c r="D12" t="s">
+        <v>312</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>217</v>
+      </c>
+      <c r="C18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C24" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>231</v>
+      </c>
+      <c r="B27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>217</v>
+      </c>
+      <c r="C30" t="s">
+        <v>218</v>
+      </c>
+      <c r="D30" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>229</v>
+      </c>
+      <c r="C31" t="s">
+        <v>230</v>
+      </c>
+      <c r="D31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>234</v>
+      </c>
+      <c r="B33" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>217</v>
+      </c>
+      <c r="C36" t="s">
+        <v>218</v>
+      </c>
+      <c r="D36" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" t="s">
+        <v>230</v>
+      </c>
+      <c r="D37" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>217</v>
+      </c>
+      <c r="C41" t="s">
+        <v>218</v>
+      </c>
+      <c r="D41" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>161</v>
+      </c>
+      <c r="B43" t="s">
+        <v>239</v>
+      </c>
+      <c r="C43" t="s">
+        <v>240</v>
+      </c>
+      <c r="D43" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>242</v>
+      </c>
+      <c r="B45" t="s">
+        <v>243</v>
+      </c>
+      <c r="C45" t="s">
+        <v>244</v>
+      </c>
+      <c r="D45" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>246</v>
+      </c>
+      <c r="B47" t="s">
+        <v>247</v>
+      </c>
+      <c r="C47" t="s">
+        <v>248</v>
+      </c>
+      <c r="D47" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>250</v>
+      </c>
+      <c r="B48" t="s">
+        <v>247</v>
+      </c>
+      <c r="C48" t="s">
+        <v>248</v>
+      </c>
+      <c r="D48" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>252</v>
+      </c>
+      <c r="B49" t="s">
+        <v>247</v>
+      </c>
+      <c r="C49" t="s">
+        <v>248</v>
+      </c>
+      <c r="D49" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>254</v>
+      </c>
+      <c r="B50" t="s">
+        <v>247</v>
+      </c>
+      <c r="C50" t="s">
+        <v>248</v>
+      </c>
+      <c r="D50" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" t="s">
+        <v>256</v>
+      </c>
+      <c r="C52" t="s">
+        <v>257</v>
+      </c>
+      <c r="D52" t="s">
+        <v>258</v>
+      </c>
+      <c r="E52" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>260</v>
+      </c>
+      <c r="B53" t="s">
+        <v>261</v>
+      </c>
+      <c r="C53" t="s">
+        <v>262</v>
+      </c>
+      <c r="D53" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>264</v>
+      </c>
+      <c r="B55" t="s">
+        <v>265</v>
+      </c>
+      <c r="C55" t="s">
+        <v>266</v>
+      </c>
+      <c r="D55" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
@@ -11668,7 +12842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -11731,6 +12905,334 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>11</v>
+      </c>
+      <c r="B10" s="13">
+        <v>12</v>
+      </c>
+      <c r="C10" s="13">
+        <v>13</v>
+      </c>
+      <c r="D10" s="13">
+        <v>14</v>
+      </c>
+      <c r="E10" s="13">
+        <v>15</v>
+      </c>
+      <c r="F10" s="13">
+        <v>16</v>
+      </c>
+      <c r="G10" s="13">
+        <v>17</v>
+      </c>
+      <c r="H10" s="13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B20" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" s="16">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>129</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2">
+        <v>42056</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>130</v>
+      </c>
+      <c r="B3">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3">
+        <v>42080</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>130</v>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4">
+        <v>42080</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>131</v>
+      </c>
+      <c r="B5">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5">
+        <v>42070</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>131</v>
+      </c>
+      <c r="B6">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6">
+        <v>42070</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>

</xml_diff>